<commit_message>
chapter 6 expample 7&8&9
</commit_message>
<xml_diff>
--- a/src/Chapter-6/案例08 使用方差分析对比数据的差异/方差分析.xlsx
+++ b/src/Chapter-6/案例08 使用方差分析对比数据的差异/方差分析.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\超简单：使用Python让Excel飞起来\代码文件\06\使用方差分析检验因素的影响力\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MGF\Documents\GitHub\TianXiaPy\PyExcel\src\Chapter-6\案例08 使用方差分析对比数据的差异\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC67E039-B567-4F5B-A1AC-17C8AB93D10C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C58DA5F-649F-4BCF-9A47-A8DB97890F6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="单因素方差分析" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>A型号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,60 @@
                 刹车距离
 汽车序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>A型号</t>
+  </si>
+  <si>
+    <t>B型号</t>
+  </si>
+  <si>
+    <t>C型号</t>
+  </si>
+  <si>
+    <t>D型号</t>
+  </si>
+  <si>
+    <t>E型号</t>
+  </si>
+  <si>
+    <t>方差分析</t>
+  </si>
+  <si>
+    <t>sum_sq</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>PR(&gt;F)</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>C(Threat)</t>
+  </si>
+  <si>
+    <t>Residual</t>
   </si>
 </sst>
 </file>
@@ -126,7 +180,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -143,6 +197,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -540,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
@@ -554,7 +611,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -574,7 +631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -593,8 +650,32 @@
       <c r="F2" s="2">
         <v>295</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -613,8 +694,35 @@
       <c r="F3" s="2">
         <v>294</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <v>274.39999999999998</v>
+      </c>
+      <c r="K3" s="1">
+        <v>6.6030296076876711</v>
+      </c>
+      <c r="L3" s="1">
+        <v>265</v>
+      </c>
+      <c r="M3" s="1">
+        <v>268.75</v>
+      </c>
+      <c r="N3" s="1">
+        <v>273.5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>279.75</v>
+      </c>
+      <c r="P3" s="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -633,8 +741,35 @@
       <c r="F4" s="2">
         <v>290</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>282.89999999999998</v>
+      </c>
+      <c r="K4" s="1">
+        <v>27.79868102386634</v>
+      </c>
+      <c r="L4" s="1">
+        <v>263</v>
+      </c>
+      <c r="M4" s="1">
+        <v>268.75</v>
+      </c>
+      <c r="N4" s="1">
+        <v>277</v>
+      </c>
+      <c r="O4" s="1">
+        <v>283.25</v>
+      </c>
+      <c r="P4" s="1">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -653,8 +788,35 @@
       <c r="F5" s="2">
         <v>287</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
+        <v>262.7</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.6184220797895446</v>
+      </c>
+      <c r="L5" s="1">
+        <v>254</v>
+      </c>
+      <c r="M5" s="1">
+        <v>259</v>
+      </c>
+      <c r="N5" s="1">
+        <v>261.5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>267.75</v>
+      </c>
+      <c r="P5" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -673,8 +835,35 @@
       <c r="F6" s="2">
         <v>268</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
+        <v>268</v>
+      </c>
+      <c r="K6" s="1">
+        <v>10.934146311237816</v>
+      </c>
+      <c r="L6" s="1">
+        <v>258</v>
+      </c>
+      <c r="M6" s="1">
+        <v>261</v>
+      </c>
+      <c r="N6" s="1">
+        <v>262.5</v>
+      </c>
+      <c r="O6" s="1">
+        <v>270.75</v>
+      </c>
+      <c r="P6" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -693,8 +882,35 @@
       <c r="F7" s="2">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <v>285</v>
+      </c>
+      <c r="K7" s="1">
+        <v>12.092238098144703</v>
+      </c>
+      <c r="L7" s="1">
+        <v>259</v>
+      </c>
+      <c r="M7" s="1">
+        <v>284.75</v>
+      </c>
+      <c r="N7" s="1">
+        <v>288.5</v>
+      </c>
+      <c r="O7" s="1">
+        <v>293.25</v>
+      </c>
+      <c r="P7" s="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -714,7 +930,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -734,7 +950,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -754,7 +970,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -774,7 +990,71 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="H14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="I15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="H16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1">
+        <v>752953.60000000114</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>3380.3811082068014</v>
+      </c>
+      <c r="L16" s="1">
+        <v>5.5207908951615785E-44</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.15">
+      <c r="H17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3622.599999999989</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1">
+        <v>4.0659107688009932</v>
+      </c>
+      <c r="L17" s="1">
+        <v>6.7397238407765434E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.15">
+      <c r="H18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="1">
+        <v>10023.4</v>
+      </c>
+      <c r="J18" s="1">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>